<commit_message>
update the weekly weight, need to fix axis for secondary addition
</commit_message>
<xml_diff>
--- a/weights.xlsx
+++ b/weights.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E99"/>
+  <dimension ref="A1:E104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
       <selection activeCell="D91" sqref="D91"/>
@@ -1919,6 +1919,93 @@
         <v>184</v>
       </c>
       <c r="C99" t="inlineStr">
+        <is>
+          <t>Marat</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>2025-10-13</t>
+        </is>
+      </c>
+      <c r="B100" t="n">
+        <v>197</v>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Marat</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>2025-10-13</t>
+        </is>
+      </c>
+      <c r="B101" t="n">
+        <v>207.1</v>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Michael</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>14.94</v>
+      </c>
+      <c r="E101" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>2025-10-20</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
+        <v>199.8</v>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>Marat</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>2025-10-27</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>209.5</v>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>Michael</t>
+        </is>
+      </c>
+      <c r="D103" t="n">
+        <v>15.38</v>
+      </c>
+      <c r="E103" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>2025-10-28</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>201.2</v>
+      </c>
+      <c r="C104" t="inlineStr">
         <is>
           <t>Marat</t>
         </is>

</xml_diff>